<commit_message>
#186 Added git hook that updates project version on post commit.
- Updated gant chart.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Online\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74065F9-7E61-4653-895A-72EB5B9A62B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0516959C-16AE-4381-B4A1-0168E6F716EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="18120" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -209,10 +209,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Main Board'!$A$2:$A$7</c:f>
+              <c:f>'Main Board'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -227,16 +227,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Main Board'!$C$2:$C$7</c:f>
+              <c:f>'Main Board'!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -250,6 +256,12 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
@@ -288,10 +300,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Main Board'!$A$2:$A$7</c:f>
+              <c:f>'Main Board'!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -306,16 +318,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44950</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Main Board'!$B$2:$B$7</c:f>
+              <c:f>'Main Board'!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -330,6 +348,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1089,13 +1113,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117021</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>631371</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1421,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1498,15 +1522,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="7">
+        <v>44950</v>
+      </c>
+      <c r="B7">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="7">
+        <v>44951</v>
+      </c>
+      <c r="B8">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#186 Moved git post commit hook to auto versioning plugin project because it mostly works with that.
- Updated gant chart.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Online\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0516959C-16AE-4381-B4A1-0168E6F716EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B583848-5043-44BF-9298-3CFD16BCB2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="18120" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -353,7 +353,7 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1448,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1538,10 +1538,10 @@
         <v>44951</v>
       </c>
       <c r="B8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
#210 Updated to UE 5.3.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8B0D5D-39D0-46D8-98BB-9354BACF5094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1A3D01-066F-4CFB-A707-6AF90A78671D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
@@ -301,6 +301,13 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Main Board'!$A$2:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>'Main Board'!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
@@ -401,11 +408,21 @@
                 <c:pt idx="31">
                   <c:v>45185</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>45186</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Main Board'!$C$2:$C$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>'Main Board'!$C$2:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -505,6 +522,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -542,6 +562,13 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Main Board'!$A$2:$A$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>'Main Board'!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
@@ -642,11 +669,21 @@
                 <c:pt idx="31">
                   <c:v>45185</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>45186</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Main Board'!$B$2:$B$35</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>'Main Board'!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -746,6 +783,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1505,13 +1545,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1837,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1897,11 +1937,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D33" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D34" si="0" xml:space="preserve"> B3 + C3</f>
         <v>48</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E33" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E34" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20833333333333334</v>
       </c>
     </row>
@@ -2475,17 +2515,36 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="8"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" s="7">
+        <v>45186</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>35</v>
+      </c>
+      <c r="D34" s="13">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="E34" s="9">
+        <f t="shared" si="1"/>
+        <v>0.51470588235294112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="8"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated gant chart and incremented version.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1805AE-B670-4DD7-BCA1-F826AA670618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B206ED-ED6F-491B-BB1D-1D50BD249EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="4180" windowWidth="28800" windowHeight="15370" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
+    <workbookView xWindow="5600" yWindow="5370" windowWidth="28800" windowHeight="15370" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$31</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$32</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$30</c:f>
+              <c:f>'Main Board'!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -398,6 +398,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45379</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,14 +410,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$31</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$32</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$30</c:f>
+              <c:f>'Main Board'!$C$2:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -501,6 +504,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -541,14 +547,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$31</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$32</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$30</c:f>
+              <c:f>'Main Board'!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -635,6 +641,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>45379</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,14 +653,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$31</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$32</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$30</c:f>
+              <c:f>'Main Board'!$B$2:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -738,6 +747,9 @@
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1498,13 +1510,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1830,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1890,11 +1902,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D30" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D31" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E30" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E31" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2411,17 +2423,36 @@
         <v>0.65151515151515149</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="7">
+        <v>45383</v>
+      </c>
+      <c r="B31">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>44</v>
+      </c>
+      <c r="D31" s="13">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="E31" s="9">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="8"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commiting updated gant chart
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B206ED-ED6F-491B-BB1D-1D50BD249EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFC8500-4AA4-428C-93F5-91EC5EA8A43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="5370" windowWidth="28800" windowHeight="15370" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$32</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$33</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$31</c:f>
+              <c:f>'Main Board'!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -401,6 +401,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45383</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,14 +413,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$32</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$33</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$31</c:f>
+              <c:f>'Main Board'!$C$2:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -507,6 +510,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -547,14 +553,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$32</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$33</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$31</c:f>
+              <c:f>'Main Board'!$A$2:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -644,6 +650,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>45383</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -653,14 +662,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$32</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$33</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$31</c:f>
+              <c:f>'Main Board'!$B$2:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -750,6 +759,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1510,13 +1522,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1842,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1902,11 +1914,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D31" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D32" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E31" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E32" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2442,17 +2454,36 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="7">
+        <v>45431</v>
+      </c>
+      <c r="B32">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <v>45</v>
+      </c>
+      <c r="D32" s="13">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="E32" s="9">
+        <f t="shared" si="1"/>
+        <v>0.68181818181818177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="8"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated gant chart and removed auto versioning editor blueprint.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B815F40-550E-43DD-9892-DAA694D94B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3FA136-34D7-4E4A-B7C1-1F571F826D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
+    <workbookView xWindow="9830" yWindow="0" windowWidth="19830" windowHeight="20970" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board" sheetId="1" r:id="rId1"/>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$34</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$35</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$33</c:f>
+              <c:f>'Main Board'!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -407,6 +407,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>45437</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -416,14 +419,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$34</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$35</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$33</c:f>
+              <c:f>'Main Board'!$C$2:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -519,6 +522,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,14 +565,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$34</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$35</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$33</c:f>
+              <c:f>'Main Board'!$A$2:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -662,6 +668,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>45437</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,14 +680,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$34</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$35</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$33</c:f>
+              <c:f>'Main Board'!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -773,6 +782,9 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -1534,13 +1546,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1866,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1926,11 +1938,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D33" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D34" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E33" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E34" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2504,17 +2516,36 @@
         <v>0.69696969696969702</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="7">
+        <v>45478</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>47</v>
+      </c>
+      <c r="D34" s="13">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="E34" s="9">
+        <f t="shared" si="1"/>
+        <v>0.70149253731343286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="8"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed auto versioning plugin and updated gant chart and versioning tool settings.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44117FD-6B13-4116-896F-19D1784681B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B0DE87-E87A-4B0A-B911-7D8A72311408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$36</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$38</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$35</c:f>
+              <c:f>'Main Board'!$A$2:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -413,6 +413,12 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>45506</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45510</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,14 +428,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$36</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$38</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$35</c:f>
+              <c:f>'Main Board'!$C$2:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -531,6 +537,12 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -571,14 +583,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$36</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$38</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$35</c:f>
+              <c:f>'Main Board'!$A$2:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -680,6 +692,12 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>45506</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45510</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45515</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,14 +707,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$36</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$38</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$35</c:f>
+              <c:f>'Main Board'!$B$2:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -798,6 +816,12 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1558,13 +1582,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1890,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1950,11 +1974,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D35" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D37" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E35" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E37" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2566,17 +2590,55 @@
         <v>0.73529411764705888</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="7">
+        <v>45510</v>
+      </c>
+      <c r="B36">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>53</v>
+      </c>
+      <c r="D36" s="13">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E36" s="9">
+        <f t="shared" si="1"/>
+        <v>0.75714285714285712</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="7">
+        <v>45515</v>
+      </c>
+      <c r="B37">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <v>55</v>
+      </c>
+      <c r="D37" s="13">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="E37" s="9">
+        <f t="shared" si="1"/>
+        <v>0.77464788732394363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="8"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#167 Setup a PvP volume for practice area.
- Fixed broken main menu when returning from lobby.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B0DE87-E87A-4B0A-B911-7D8A72311408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882CE65C-98D8-4C4F-9A19-439C8348E2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$38</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$39</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$37</c:f>
+              <c:f>'Main Board'!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -419,6 +419,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>45515</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -428,14 +431,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$38</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$39</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$37</c:f>
+              <c:f>'Main Board'!$C$2:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -543,6 +546,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -583,14 +589,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$38</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$39</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$37</c:f>
+              <c:f>'Main Board'!$A$2:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -698,6 +704,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>45515</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -707,14 +716,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$38</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$39</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$37</c:f>
+              <c:f>'Main Board'!$B$2:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -822,6 +831,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1582,13 +1594,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1914,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1974,11 +1986,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D37" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D38" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E37" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E38" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2628,17 +2640,36 @@
         <v>0.77464788732394363</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="7">
+        <v>45540</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>56</v>
+      </c>
+      <c r="D38" s="13">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="E38" s="9">
+        <f t="shared" si="1"/>
+        <v>0.78873239436619713</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="8"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#229 Removed own plugin with the old project version getter.
- Updated gant chart.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AF63C0-8E75-4FAC-8762-F517910AC406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF5E37D-5B4B-4A0D-B40E-5AE81D939B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$40</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$41</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$39</c:f>
+              <c:f>'Main Board'!$A$2:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -425,6 +425,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>45543</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -434,14 +437,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$40</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$41</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$39</c:f>
+              <c:f>'Main Board'!$C$2:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -555,6 +558,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,14 +601,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$40</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$41</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$39</c:f>
+              <c:f>'Main Board'!$A$2:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -716,6 +722,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>45543</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,14 +734,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$40</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$41</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$39</c:f>
+              <c:f>'Main Board'!$B$2:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -846,6 +855,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1606,13 +1618,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1938,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1998,11 +2010,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D39" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D40" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E39" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E40" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2690,17 +2702,36 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="8"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="11"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="7">
+        <v>1020</v>
+      </c>
+      <c r="B40">
+        <v>18</v>
+      </c>
+      <c r="C40">
+        <v>57</v>
+      </c>
+      <c r="D40" s="13">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="E40" s="9">
+        <f t="shared" si="1"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="8"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated gant chart and commited lingering change.
</commit_message>
<xml_diff>
--- a/gantChart.xlsx
+++ b/gantChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Games\UEFPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6526822-11B1-4E3C-A8D6-2A52EC0ADF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB3DF70-8D95-49DA-9C04-2E1642B6A476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{28D99B71-C0F5-45BA-8373-277E5ED99469}"/>
   </bookViews>
@@ -304,14 +304,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$43</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$44</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$42</c:f>
+              <c:f>'Main Board'!$A$2:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -434,6 +434,9 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>45605</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -443,14 +446,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$C$2:$C$43</c15:sqref>
+                    <c15:sqref>'Main Board'!$C$2:$C$44</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$C$2:$C$42</c:f>
+              <c:f>'Main Board'!$C$2:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -573,6 +576,9 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,14 +619,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$A$2:$A$43</c15:sqref>
+                    <c15:sqref>'Main Board'!$A$2:$A$44</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$A$2:$A$42</c:f>
+              <c:f>'Main Board'!$A$2:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm\-yy;@</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>44944</c:v>
                 </c:pt>
@@ -743,6 +749,9 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>45605</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,14 +761,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>'Main Board'!$B$2:$B$43</c15:sqref>
+                    <c15:sqref>'Main Board'!$B$2:$B$44</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>'Main Board'!$B$2:$B$42</c:f>
+              <c:f>'Main Board'!$B$2:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>38</c:v>
                 </c:pt>
@@ -882,6 +891,9 @@
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1642,14 +1654,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117022</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>48985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>527958</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>16328</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1974,10 +1986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11762E8-6472-452A-80EF-BCA0E65D4CA0}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2034,11 +2046,11 @@
         <v>10</v>
       </c>
       <c r="D3" s="13">
-        <f t="shared" ref="D3:D42" si="0" xml:space="preserve"> B3 + C3</f>
+        <f t="shared" ref="D3:D43" si="0" xml:space="preserve"> B3 + C3</f>
         <v>49</v>
       </c>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E42" si="1" xml:space="preserve"> C3 / D3</f>
+        <f t="shared" ref="E3:E43" si="1" xml:space="preserve"> C3 / D3</f>
         <v>0.20408163265306123</v>
       </c>
     </row>
@@ -2783,17 +2795,36 @@
         <v>0.76315789473684215</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="8"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="7">
+        <v>45647</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>61</v>
+      </c>
+      <c r="D43" s="13">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="E43" s="9">
+        <f t="shared" si="1"/>
+        <v>0.88405797101449279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="8"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>